<commit_message>
Added code used for historical price extraction, and the resulting historical prices
</commit_message>
<xml_diff>
--- a/output/target_stock_universe.xlsx
+++ b/output/target_stock_universe.xlsx
@@ -465,20 +465,17 @@
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve">Market Cap
-</t>
+          <t>Market Cap</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve">SEDOL
-</t>
+          <t>SEDOL</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve">ISIN
-</t>
+          <t>ISIN</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
@@ -1899,20 +1896,17 @@
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve">Market Cap
-</t>
+          <t>Market Cap</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve">SEDOL
-</t>
+          <t>SEDOL</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve">ISIN
-</t>
+          <t>ISIN</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
@@ -3333,20 +3327,17 @@
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve">Market Cap
-</t>
+          <t>Market Cap</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve">SEDOL
-</t>
+          <t>SEDOL</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve">ISIN
-</t>
+          <t>ISIN</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
@@ -4767,20 +4758,17 @@
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve">Market Cap
-</t>
+          <t>Market Cap</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve">SEDOL
-</t>
+          <t>SEDOL</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve">ISIN
-</t>
+          <t>ISIN</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
@@ -6201,20 +6189,17 @@
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve">Market Cap
-</t>
+          <t>Market Cap</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve">SEDOL
-</t>
+          <t>SEDOL</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve">ISIN
-</t>
+          <t>ISIN</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">

</xml_diff>